<commit_message>
Revise based on demo with Danilo
</commit_message>
<xml_diff>
--- a/results/real_support_fte_table.xlsx
+++ b/results/real_support_fte_table.xlsx
@@ -451,7 +451,7 @@
         <v>8079.367383867557</v>
       </c>
       <c r="G2">
-        <v>7846.184410194463</v>
+        <v>7846.184410194464</v>
       </c>
       <c r="H2">
         <v>8032.026720712742</v>
@@ -503,7 +503,7 @@
         <v>21058.5386311806</v>
       </c>
       <c r="I3">
-        <v>21669.41524614916</v>
+        <v>21669.41524614917</v>
       </c>
       <c r="J3">
         <v>20847.77399423357</v>
@@ -583,7 +583,7 @@
         <v>9407.909519911582</v>
       </c>
       <c r="E5">
-        <v>9324.821468081303</v>
+        <v>9324.821468081304</v>
       </c>
       <c r="F5">
         <v>9128.629313594694</v>
@@ -656,7 +656,7 @@
         <v>10149.30298708802</v>
       </c>
       <c r="N6">
-        <v>973.7333546342797</v>
+        <v>973.7333546342798</v>
       </c>
     </row>
     <row r="7">
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>9099.555581428292</v>
+        <v>9099.555581428293</v>
       </c>
       <c r="C9">
         <v>8984.85751374772</v>
@@ -865,7 +865,7 @@
         <v>7974.783158969886</v>
       </c>
       <c r="G11">
-        <v>8126.472106184106</v>
+        <v>8126.472106184107</v>
       </c>
       <c r="H11">
         <v>8673.133890411771</v>
@@ -917,7 +917,7 @@
         <v>14178.72758061164</v>
       </c>
       <c r="I12">
-        <v>15688.65053728773</v>
+        <v>15688.65053728774</v>
       </c>
       <c r="J12">
         <v>16749.75620856343</v>
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>11115.8676864869</v>
+        <v>11115.86768648691</v>
       </c>
       <c r="C13">
         <v>11128.34249496275</v>
@@ -1018,7 +1018,7 @@
         <v>14339.86439953229</v>
       </c>
       <c r="L14">
-        <v>13193.1916606816</v>
+        <v>13193.19166068161</v>
       </c>
       <c r="M14">
         <v>13702.32109955854</v>
@@ -1144,7 +1144,7 @@
         <v>6236.895376729751</v>
       </c>
       <c r="H17">
-        <v>6026.714775867988</v>
+        <v>6026.714775867989</v>
       </c>
       <c r="I17">
         <v>6324.339824311976</v>
@@ -1196,7 +1196,7 @@
         <v>8327.030389979953</v>
       </c>
       <c r="J18">
-        <v>8397.998423656732</v>
+        <v>8397.998423656733</v>
       </c>
       <c r="K18">
         <v>8296.938836722455</v>
@@ -1221,7 +1221,7 @@
         <v>11521.07382577725</v>
       </c>
       <c r="C19">
-        <v>11017.75760187447</v>
+        <v>11017.75760187448</v>
       </c>
       <c r="D19">
         <v>9809.04954527384</v>
@@ -1331,7 +1331,7 @@
         <v>7986.564798280027</v>
       </c>
       <c r="I21">
-        <v>8291.912261534831</v>
+        <v>8291.912261534832</v>
       </c>
       <c r="J21">
         <v>8502.442710658253</v>
@@ -1500,7 +1500,7 @@
         <v>9672.213769548929</v>
       </c>
       <c r="D25">
-        <v>9897.735999983784</v>
+        <v>9897.735999983785</v>
       </c>
       <c r="E25">
         <v>8364.628689836867</v>
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>6579.929719144397</v>
+        <v>6579.929719144398</v>
       </c>
       <c r="C27">
         <v>6810.497598866056</v>
@@ -1610,7 +1610,7 @@
         <v>6669.967586196976</v>
       </c>
       <c r="J27">
-        <v>7294.418499120507</v>
+        <v>7294.418499120508</v>
       </c>
       <c r="K27">
         <v>6827.318580727449</v>
@@ -1641,7 +1641,7 @@
         <v>9058.332560860861</v>
       </c>
       <c r="E28">
-        <v>8828.120071267032</v>
+        <v>8828.120071267033</v>
       </c>
       <c r="F28">
         <v>8652.400629772283</v>
@@ -1668,7 +1668,7 @@
         <v>10041.124214851</v>
       </c>
       <c r="N28">
-        <v>22.7570067621109</v>
+        <v>22.75700676211091</v>
       </c>
     </row>
     <row r="29">
@@ -1975,10 +1975,10 @@
         <v>11992.96874269268</v>
       </c>
       <c r="I35">
-        <v>12013.33570158181</v>
+        <v>12013.33570158182</v>
       </c>
       <c r="J35">
-        <v>11951.99194927418</v>
+        <v>11951.99194927419</v>
       </c>
       <c r="K35">
         <v>12244.87502153532</v>
@@ -2012,7 +2012,7 @@
         <v>5643.934739303356</v>
       </c>
       <c r="F36">
-        <v>5304.323981319038</v>
+        <v>5304.323981319039</v>
       </c>
       <c r="G36">
         <v>5622.908049044446</v>
@@ -2049,7 +2049,7 @@
         <v>9970.397686681048</v>
       </c>
       <c r="C37">
-        <v>10135.8336699653</v>
+        <v>10135.83366996531</v>
       </c>
       <c r="D37">
         <v>9844.083981836377</v>
@@ -2064,7 +2064,7 @@
         <v>7967.688269726913</v>
       </c>
       <c r="H37">
-        <v>7832.605239668625</v>
+        <v>7832.605239668626</v>
       </c>
       <c r="I37">
         <v>8350.281415734527</v>
@@ -2095,7 +2095,7 @@
         <v>6664.496997884313</v>
       </c>
       <c r="C38">
-        <v>6271.146042191172</v>
+        <v>6271.146042191173</v>
       </c>
       <c r="D38">
         <v>5070.473897696972</v>
@@ -2119,7 +2119,7 @@
         <v>5733.9786046804</v>
       </c>
       <c r="K38">
-        <v>5909.132681000297</v>
+        <v>5909.132681000298</v>
       </c>
       <c r="L38">
         <v>6090.43031868465</v>
@@ -2165,7 +2165,7 @@
         <v>5008.697678991885</v>
       </c>
       <c r="K39">
-        <v>5064.36930081333</v>
+        <v>5064.369300813331</v>
       </c>
       <c r="L39">
         <v>5063.67467121333</v>
@@ -2208,7 +2208,7 @@
         <v>5899.585409979803</v>
       </c>
       <c r="J40">
-        <v>6229.420201692737</v>
+        <v>6229.420201692738</v>
       </c>
       <c r="K40">
         <v>6508.08701926749</v>
@@ -2282,7 +2282,7 @@
         <v>7682.900862037866</v>
       </c>
       <c r="D42">
-        <v>7221.851627679835</v>
+        <v>7221.851627679836</v>
       </c>
       <c r="E42">
         <v>6723.56642264338</v>
@@ -2521,7 +2521,7 @@
         <v>5565.583462915233</v>
       </c>
       <c r="G47">
-        <v>5872.526503544615</v>
+        <v>5872.526503544616</v>
       </c>
       <c r="H47">
         <v>6049.117254746671</v>
@@ -2558,7 +2558,7 @@
         <v>9129.549051116366</v>
       </c>
       <c r="D48">
-        <v>7714.038528636122</v>
+        <v>7714.038528636123</v>
       </c>
       <c r="E48">
         <v>6939.534522319962</v>
@@ -2567,7 +2567,7 @@
         <v>5983.188299247567</v>
       </c>
       <c r="G48">
-        <v>6230.333514722623</v>
+        <v>6230.333514722624</v>
       </c>
       <c r="H48">
         <v>6930.247600794143</v>
@@ -2690,7 +2690,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>14999.50307016741</v>
+        <v>14999.50307016742</v>
       </c>
       <c r="C51">
         <v>16547.73615627726</v>
@@ -2754,7 +2754,7 @@
         <v>7094.626943089254</v>
       </c>
       <c r="H52">
-        <v>7478.215893751169</v>
+        <v>7478.21589375117</v>
       </c>
       <c r="I52">
         <v>7914.474595788968</v>

</xml_diff>